<commit_message>
Animation and form validation have been successfully added.
</commit_message>
<xml_diff>
--- a/public/form-submissions.xlsx
+++ b/public/form-submissions.xlsx
@@ -31,19 +31,19 @@
     <t>Referral</t>
   </si>
   <si>
-    <t>Aman singh</t>
+    <t>Nikk Dwivedi</t>
   </si>
   <si>
     <t>virendraiaf18@gmail.com</t>
   </si>
   <si>
-    <t>08319693453</t>
-  </si>
-  <si>
-    <t>I'm Recruiting</t>
-  </si>
-  <si>
-    <t>python</t>
+    <t>8319693453</t>
+  </si>
+  <si>
+    <t>I'm a Developer</t>
+  </si>
+  <si>
+    <t>angular</t>
   </si>
   <si>
     <t>therighthire</t>

</xml_diff>